<commit_message>
flow v10.0.1 including tv v9.6
</commit_message>
<xml_diff>
--- a/en.xlsx
+++ b/en.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_mesDocs\_git\trouble_shooting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apeter\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="767" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" tabRatio="958" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Validators" sheetId="13" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <definedName name="salttv_en" localSheetId="2">salttv_en!$A$1:$H$1</definedName>
     <definedName name="stability_en" localSheetId="4">stability_en!$A$1:$H$23</definedName>
     <definedName name="validator_en" localSheetId="0">Validators!$A$1:$F$4</definedName>
-    <definedName name="wifi_lan_en" localSheetId="3">'wifi-lan_en'!$A$1:$H$30</definedName>
+    <definedName name="wifi_lan_en" localSheetId="3">'wifi-lan_en'!$A$1:$H$28</definedName>
   </definedNames>
   <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="894">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="890">
   <si>
     <t>FLAG</t>
   </si>
@@ -2126,12 +2126,6 @@
     <t>$flow.lan.OkToTryWifi</t>
   </si>
   <si>
-    <t>Ok let's go</t>
-  </si>
-  <si>
-    <t>No, cannot do</t>
-  </si>
-  <si>
     <t>box/lan/switch</t>
   </si>
   <si>
@@ -2144,33 +2138,18 @@
     <t>box/lan/lan_ok</t>
   </si>
   <si>
-    <t>Have the customer openening a browser and enter google.com&lt;N&gt;If he can reach it than no ticket will be created &lt;b&gt;unless the client states the url or app&lt;b&gt; that still doesn't work.</t>
-  </si>
-  <si>
-    <t>In the majority of cases the customer has WiFi devices and it will be very useful to try.&lt;N&gt;In other cases either the customer has no WiFi device or he asserts it is working fine with WiFi, select NO then a LAN ISSUE ticket will be created.</t>
-  </si>
-  <si>
     <t>Get close to the box and make sure you are not within the range of a WiFi repeater</t>
   </si>
   <si>
     <t>Test Google and then other URLs on the device's browser</t>
   </si>
   <si>
-    <t>Now let's try to see if it works on WiFi</t>
-  </si>
-  <si>
     <t>No connection at all</t>
   </si>
   <si>
     <t>Can see Google but no other URLs</t>
   </si>
   <si>
-    <t>Read the optimal WiFi advices page and send a link to the customer.</t>
-  </si>
-  <si>
-    <t>Request the client to do/use/start again what led him to call us&lt;N&gt;&lt;T&gt;- Streaming app freezing&lt;N&gt;&lt;T&gt;- Long page loading&lt;N&gt;&lt;T&gt;- Etc.</t>
-  </si>
-  <si>
     <t>The device is connected through an Ethernet switch ?</t>
   </si>
   <si>
@@ -2354,9 +2333,6 @@
     <t>https://support.apple.com/en-gb/HT202118</t>
   </si>
   <si>
-    <t xml:space="preserve">An AppleID created by selecting a country other than Switzerland does not allow you to download SaltTV. </t>
-  </si>
-  <si>
     <t>Swiss Apple ID</t>
   </si>
   <si>
@@ -2378,9 +2354,6 @@
     <t>Not visible</t>
   </si>
   <si>
-    <t>If so, the client may be barred.</t>
-  </si>
-  <si>
     <t>Is there a message prompting the customer to call the customer care?</t>
   </si>
   <si>
@@ -2447,9 +2420,6 @@
     <t>Sign in with a Swiss Apple TV account</t>
   </si>
   <si>
-    <t>&lt;N&gt;&lt;T&gt;- Check the account to analyse the status&lt;N&gt;&lt;T&gt;- Check if there isn't any ticket opened for this case&lt;N&gt;&lt;T&gt;- Check if there is no outstanding technical issue that could be the source of the issue"</t>
-  </si>
-  <si>
     <t>$flow.tv.WhatIStheTVIssue</t>
   </si>
   <si>
@@ -2459,39 +2429,21 @@
     <t>Sound is bad</t>
   </si>
   <si>
-    <t>What issue do you face ?</t>
-  </si>
-  <si>
     <t>Can't watch TV</t>
   </si>
   <si>
-    <t>Choose remote for &lt;N&gt;&lt;T&gt;- Siri remote issues&lt;N&gt;&lt;T&gt;- Salt TV remote&lt;N&gt;&lt;N&gt;Choose TV for issue with &lt;N&gt;&lt;T&gt;- AppleTV&lt;N&gt;&lt;T&gt;- Salt TV app&lt;N&gt;&lt;T&gt;- channels &lt;N&gt;&lt;T&gt;- feature &lt;N&gt;&lt;T&gt;- install&lt;N&gt;&lt;T&gt;- Etc…</t>
-  </si>
-  <si>
     <t>$flow.tv.sound._StoreCustomersSetup</t>
   </si>
   <si>
-    <t>What is customer's setup ?</t>
-  </si>
-  <si>
     <t>&lt;N&gt;&lt;T&gt;-TV brand and model&lt;N&gt;&lt;T&gt;-Soundsystem brand and model</t>
   </si>
   <si>
     <t>$flow.tv.sound._AppleTVSoundSetup</t>
   </si>
   <si>
-    <t>How is Apple TV sound setup ?</t>
-  </si>
-  <si>
-    <t>&lt;N&gt;&lt;T&gt;-AudioOutput&lt;N&gt;&lt;T&gt;-AudioFormat&lt;N&gt;&lt;T&gt;-ReduceLoudSounds&lt;N&gt;&lt;T&gt;-AudioMode</t>
-  </si>
-  <si>
     <t>$flow.tv.sound._SaltTVDetails</t>
   </si>
   <si>
-    <t>Give us more detail on how you use Salt TV when you face sound issue ?</t>
-  </si>
-  <si>
     <t>&lt;N&gt;&lt;T&gt;-Channels impacted&lt;N&gt;&lt;T&gt;-ProgramName&lt;N&gt;&lt;T&gt;-TimeAndDate</t>
   </si>
   <si>
@@ -2501,33 +2453,18 @@
     <t>Describe the sound issue</t>
   </si>
   <si>
-    <t>What exactly is the audio defect that the customer faces</t>
-  </si>
-  <si>
     <t>$flow.tv.sound._HowFerquent</t>
   </si>
   <si>
-    <t>How frequent, when does it happen ?</t>
-  </si>
-  <si>
-    <t>Ask if the issue appears on alll channel or a single one. Always or time to time etc…</t>
-  </si>
-  <si>
     <t>$flow.tv.sound.IsSameIssueWithOtherApps</t>
   </si>
   <si>
-    <t>Does the sound issue occurs with other apps on the Apple TV ?</t>
-  </si>
-  <si>
     <t>Expl: with iTunes, Spotify, games etc...</t>
   </si>
   <si>
     <t>$flow.tv.remote.WichRemote</t>
   </si>
   <si>
-    <t>With remote is it ?</t>
-  </si>
-  <si>
     <t>Applt TV Siri remote</t>
   </si>
   <si>
@@ -2537,9 +2474,6 @@
     <t>$flow.tv.remote.DoesAppleTVLedBlinks</t>
   </si>
   <si>
-    <t>Does the light on the Apple TV lids and the icons on the TV are moving ?</t>
-  </si>
-  <si>
     <t>$flow.tv.remote.siri._RechargeSiriRemote</t>
   </si>
   <si>
@@ -2549,15 +2483,9 @@
     <t>$flow.tv.remote.siri._GetCloseToAppleTV</t>
   </si>
   <si>
-    <t>With the remote in hand get close to the Apple TV</t>
-  </si>
-  <si>
     <t>$flow.tv.remote.siri._PressMenuAndPlus</t>
   </si>
   <si>
-    <t>Bind the Siri remote to Apple TV&lt;N&gt;Press MENU and + button simoustaneously</t>
-  </si>
-  <si>
     <t>$flow.tv.remote.siri._AdviceOnSiriRemoteUSage</t>
   </si>
   <si>
@@ -2567,9 +2495,6 @@
     <t>https://fiber.salt.ch/fiber/equipment/apple-tv/guide</t>
   </si>
   <si>
-    <t>Open the Salt page.&lt;N&gt;Review the functionalities with the customer&lt;N&gt;Send the lik to the Salt Fiber Apple TV guide</t>
-  </si>
-  <si>
     <t>$flow.tv.remote.satltv._EnsureAppleTVInVisualRangeOfRemote</t>
   </si>
   <si>
@@ -2579,9 +2504,6 @@
     <t>$flow.tv.remote.satltv.DoesRedLedBlinksOnRemoteWhenPressed</t>
   </si>
   <si>
-    <t>Does the red LED blinks on the remote ?</t>
-  </si>
-  <si>
     <t>$flow.tv.remote.satltv._MakeSureBatteriesCoerrectlyInstalled</t>
   </si>
   <si>
@@ -2594,67 +2516,36 @@
     <t>$flow.tv.remote.satltv.CanReplaceBatteries</t>
   </si>
   <si>
-    <t>Can you replace the batteries now ?</t>
-  </si>
-  <si>
     <t>$flow.tv.remote.satltv._ReplaceBatteriesThenCallUsBack</t>
   </si>
   <si>
-    <t>Please replace thenm and call us back</t>
-  </si>
-  <si>
     <t>$flow.tv.remote.satltv.IsAppleTVFourthGen</t>
   </si>
   <si>
-    <t>Is the Apple TV a fourth generation one ?</t>
-  </si>
-  <si>
     <t>https://support.apple.com/HT200008</t>
   </si>
   <si>
-    <t>Open the Apple support page&lt;N&gt;Check the look and the Model number if they match the one of Apple TV 4K or Apple TV HD</t>
-  </si>
-  <si>
     <t>$flow.tv.remote.satltv.IsLatestSaltTVAppInstalled</t>
   </si>
   <si>
-    <t>Is the latestest Salt TV app installed ?</t>
-  </si>
-  <si>
     <t>$flow.tv.remote.satltv._SteupSaltTVRemoteWithRegularTV</t>
   </si>
   <si>
-    <t>Try to set up Salt TV remote with regular TV</t>
-  </si>
-  <si>
     <t>$flow.tv.remote.satltv.DoesVolumeOnTvChange</t>
   </si>
   <si>
-    <t>Does the volume onthe TV change ?</t>
-  </si>
-  <si>
     <t>$flow.tv.remote.satltv.WasThePurchaseDoneLessThanOnYearAgo</t>
   </si>
   <si>
-    <t>When did you buy the remote ?&lt;N&gt; More than a year ago ?</t>
-  </si>
-  <si>
     <t>$flow.tv.remote.satltv._GoToStoreToReplace</t>
   </si>
   <si>
     <t>Go to a store to replace it</t>
   </si>
   <si>
-    <t>Take your proof of purchase with you. Go to a Salt Store
-Remote will be replaced</t>
-  </si>
-  <si>
     <t>$flow.tv.remote.satltv._NeedToBuyOneNew</t>
   </si>
   <si>
-    <t>Warranty is passed. Seems like your remote is defect. &lt;N&gt;You would need to buy a new one.</t>
-  </si>
-  <si>
     <t>$flow.tv.hardware.IsAppleTVvisibleOnTVScreen</t>
   </si>
   <si>
@@ -2706,31 +2597,264 @@
     <t>$flow.tv.install._ResetAppleTV</t>
   </si>
   <si>
-    <t>Open the Apple store on the  Apple TV</t>
-  </si>
-  <si>
-    <t>Can you see Salt TV on the store</t>
-  </si>
-  <si>
-    <t>Type Salt on the search</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you have an Apple ID (Apple account) </t>
-  </si>
-  <si>
-    <t>Are you ok to create one ?</t>
-  </si>
-  <si>
-    <t>Take the time with the customer to help him create the Apple ID.&lt;N&gt;Make sure to select Swiss as a country.</t>
+    <t>Find the LEX and OLT in VTI, compare with the list of service incidents in Qoof</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Now let's try to see if it works with a WiFi </t>
+  </si>
+  <si>
+    <t>WiFi works</t>
+  </si>
+  <si>
+    <t>Doesn't work neither on WiFi</t>
+  </si>
+  <si>
+    <t>did not test WiFi</t>
+  </si>
+  <si>
+    <t>In the majority of cases the customer has WiFi devices and it will be very useful to know .&lt;N&gt; Just ask the customer to connect to the  WiFi with an device.</t>
+  </si>
+  <si>
+    <t>Let's try to test with the AppleTV in LAN.</t>
+  </si>
+  <si>
+    <t>Cannot use Apple TV with LAN</t>
+  </si>
+  <si>
+    <t>Let's try with another device in LAN.</t>
+  </si>
+  <si>
+    <t>No other LAN device available</t>
+  </si>
+  <si>
+    <t>All set let's test</t>
+  </si>
+  <si>
+    <t>$flow.tv.app._QuitAndRelaunchSaltTV</t>
+  </si>
+  <si>
+    <t>$flow.tv.app.ProblemSolved</t>
+  </si>
+  <si>
+    <t>$flow.tv.app._CheckIfAppNeedsUpdate</t>
+  </si>
+  <si>
+    <t>$flow.tv.app._RebootAppleTV</t>
+  </si>
+  <si>
+    <t>$flow.tv.app._CheckIfSaltTVNeedsUpdate</t>
+  </si>
+  <si>
+    <t>$flow.tv.app.WhatAppleTVcnxType</t>
+  </si>
+  <si>
+    <t>$flow.tv.app.IsIssueWithOtherApps</t>
+  </si>
+  <si>
+    <t>$flow.tv.app.CanCheckWithLan</t>
+  </si>
+  <si>
+    <t>$flow.tv.services.IsMessageInvitingToContactCC</t>
+  </si>
+  <si>
+    <t>$flow.tv.services.IsTVServicesActiveVTI</t>
+  </si>
+  <si>
+    <t>$flow.tv.services.IsBasicTvPackageVisible</t>
+  </si>
+  <si>
+    <t>$flow.tv.services.IsBarringVisible</t>
+  </si>
+  <si>
+    <t>$flow.tv._OpenSaltTVApp</t>
+  </si>
+  <si>
+    <t>$flow.tv.CanExploreMenu</t>
+  </si>
+  <si>
+    <t>$flow.tv._InformSaltIsFixing</t>
+  </si>
+  <si>
+    <t>Can you explore the Salt TV menu ?</t>
+  </si>
+  <si>
+    <t>$flow.tv.ChekSaltTVKNownBugs</t>
+  </si>
+  <si>
+    <t>Yes there is incident</t>
+  </si>
+  <si>
+    <t>Our technician are fixing it.</t>
+  </si>
+  <si>
+    <t>Check in VTI if the customer has basic packages</t>
+  </si>
+  <si>
+    <t>Check in VTI if any barring is visible</t>
+  </si>
+  <si>
+    <t>https://support.apple.com/en-us/HT201389</t>
+  </si>
+  <si>
+    <t>Remote</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>Sound</t>
+  </si>
+  <si>
+    <t>$flow.lan.LetsCheckYourWiFi</t>
+  </si>
+  <si>
+    <t>Have the customer open a browser on a WiFi connected device and try google.com</t>
+  </si>
+  <si>
+    <t>WiFi works too</t>
+  </si>
+  <si>
+    <t>Did not work</t>
+  </si>
+  <si>
+    <t>customer/google_wifi</t>
+  </si>
+  <si>
+    <t>$flow.tv._CreateSOTicketSaltTV</t>
+  </si>
+  <si>
+    <t>A ticket [541] will be automatically generated upon advancing to the next step. Do not manually create one (SuperOffice). A copy of the content will be sent to your mailbox.</t>
+  </si>
+  <si>
+    <t>Automatic ticket creation [541] in SuperOffice</t>
+  </si>
+  <si>
+    <t>What is the customer's setup ?</t>
+  </si>
+  <si>
+    <t>Give us more detail on how you use Salt TV when you face issues with the sound?</t>
+  </si>
+  <si>
+    <t>Ask if the issue appears on all channels or a single one. Always or time to time etc…</t>
+  </si>
+  <si>
+    <t>Which remote type is used?</t>
+  </si>
+  <si>
+    <t>Does the light on the Apple TV lids and the icons on the TV are moving?</t>
+  </si>
+  <si>
+    <t>With the remote in hand get closer to the Apple TV</t>
+  </si>
+  <si>
+    <t>Point the Siri remote to Apple TV&lt;N&gt;Press MENU and + button simultaneously</t>
+  </si>
+  <si>
+    <t>Is the red LED on the remote control blinking?</t>
+  </si>
+  <si>
+    <t>How is the Apple TV sound setup?</t>
+  </si>
+  <si>
+    <t>How frequent, when does it happen?</t>
+  </si>
+  <si>
+    <t>Does the sound issue occurs with other apps on the Apple TV?</t>
+  </si>
+  <si>
+    <t>Can you replace the batteries now?</t>
+  </si>
+  <si>
+    <t>Please replace them and call us back</t>
+  </si>
+  <si>
+    <t>Is the Apple TV a fourth generation one?</t>
+  </si>
+  <si>
+    <t>Is the latest Salt TV app installed?</t>
+  </si>
+  <si>
+    <t>Try to set up the Salt TV remote with regular TV</t>
+  </si>
+  <si>
+    <t>Does the volume change on the TV?</t>
+  </si>
+  <si>
+    <t>When did you buy the remote ?&lt;N&gt; More than a year ago?</t>
+  </si>
+  <si>
+    <t>Warranty is expired. Seems like your remote is defect. &lt;N&gt;You need to buy a new one.</t>
+  </si>
+  <si>
+    <t>Open the App Store on the  Apple TV</t>
+  </si>
+  <si>
+    <t>Can you see Salt TV in the store</t>
+  </si>
+  <si>
+    <t>Do you have an Apple ID (Apple account)?</t>
+  </si>
+  <si>
+    <t>Are you ok to create one?</t>
+  </si>
+  <si>
+    <t>Is the Apple ID a swiss Apple ID?</t>
+  </si>
+  <si>
+    <t>Is it allright with you to change the country of your Apple ID to Swizerland?</t>
+  </si>
+  <si>
+    <t>Let's change your Apple ID country!</t>
+  </si>
+  <si>
+    <t>Does the issue occur only with Salt TV or with other Apple TV apps?</t>
+  </si>
+  <si>
+    <t>Can you try connecting the Apple TV to the LAN?</t>
+  </si>
+  <si>
+    <t>What issue do you face?</t>
+  </si>
+  <si>
+    <t>With what do  you face issues?</t>
+  </si>
+  <si>
+    <t>What exactly is the audio defect that the customer faces?</t>
+  </si>
+  <si>
+    <t>Open the Apple support page&lt;N&gt;Check if the design and the model number match the one of Apple TV 4K or Apple TV HD</t>
+  </si>
+  <si>
+    <t>Type Salt in the search field</t>
+  </si>
+  <si>
+    <t>Take the time with the customer to help him create the Apple ID.&lt;N&gt;Make sure to select Switzerland as a country.</t>
+  </si>
+  <si>
+    <t>Customer can always revert to another country if needed later.&lt;N&gt;Read "What to do before you change your country or region" on the link below to know the conditions of changing languge of an Apple ID</t>
+  </si>
+  <si>
+    <t>If so, the customer may be barred.</t>
+  </si>
+  <si>
+    <t>Choose remote for &lt;N&gt;&lt;T&gt;- Siri remote issues&lt;N&gt;&lt;T&gt;- Salt TV remote&lt;N&gt;&lt;N&gt;Choose TV for issue with &lt;N&gt;&lt;T&gt;- Apple TV&lt;N&gt;&lt;T&gt;- Salt TV app&lt;N&gt;&lt;T&gt;- channels &lt;N&gt;&lt;T&gt;- feature &lt;N&gt;&lt;T&gt;- install&lt;N&gt;&lt;T&gt;- Etc…</t>
+  </si>
+  <si>
+    <t>Channel issue = I cannot broadcast a channel&lt;N&gt; Feature issue some app funcitonality doesn not work</t>
+  </si>
+  <si>
+    <t>The LAN conection works, let's test your WiFi connection</t>
+  </si>
+  <si>
+    <t>Request the customer to do/use/start again what led him to call us&lt;N&gt;&lt;T&gt;- Streaming app freezing&lt;N&gt;&lt;T&gt;- Long page loading&lt;N&gt;&lt;T&gt;- Etc.</t>
   </si>
   <si>
     <r>
-      <t>When the problem occurs, is the device</t>
+      <t>When the problem occurs, is/are the device</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="8"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2749,178 +2873,40 @@
     </r>
   </si>
   <si>
-    <t>Find the LEX and OLT in VTI, compare with the list of service incidents in Qoof</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Now let's try to see if it works with a WiFi </t>
-  </si>
-  <si>
-    <t>WiFi works</t>
-  </si>
-  <si>
-    <t>Doesn't work neither on WiFi</t>
-  </si>
-  <si>
-    <t>did not test WiFi</t>
-  </si>
-  <si>
-    <t>In the majority of cases the customer has WiFi devices and it will be very useful to know .&lt;N&gt; Just ask the customer to connect to the  WiFi with an device.</t>
-  </si>
-  <si>
-    <t>The customer contacts us, complaining about&lt;N&gt;&lt;T&gt;- not being able to connect to the Internet&lt;N&gt;&lt;T&gt;- having trouble watching the TV.&lt;N&gt;&lt;T&gt;- hasn't received his equipment (Fiber Box).&lt;N&gt;&lt;N&gt;&lt;b&gt;To carry one with the trouble shooting, the customer must be at home and be able to physically acces the box&lt;b&gt;</t>
-  </si>
-  <si>
-    <t>Same issue</t>
-  </si>
-  <si>
-    <t>Works good now</t>
-  </si>
-  <si>
-    <t>Check google.com, try to search for something like "salt" and see if results yield.&lt;N&gt;&lt;N&gt;If the customer is computer savvy, have him also double check if the operating system show that the Ethernet connexion is ok</t>
-  </si>
-  <si>
-    <t>Let's try to test with the AppleTV in LAN.</t>
-  </si>
-  <si>
-    <t>Cannot use Apple TV with LAN</t>
-  </si>
-  <si>
-    <t>If the customer has another device that he can connect in LAN, have him connect directly to the box and the the ethernet connexion like before.</t>
-  </si>
-  <si>
-    <t>Let's try with another device in LAN.</t>
-  </si>
-  <si>
-    <t>No other LAN device available</t>
-  </si>
-  <si>
-    <t>All set let's test</t>
-  </si>
-  <si>
-    <t>$flow.tv.app._QuitAndRelaunchSaltTV</t>
-  </si>
-  <si>
-    <t>$flow.tv.app.ProblemSolved</t>
-  </si>
-  <si>
-    <t>$flow.tv.app._CheckIfAppNeedsUpdate</t>
-  </si>
-  <si>
-    <t>$flow.tv.app._RebootAppleTV</t>
-  </si>
-  <si>
-    <t>$flow.tv.app._CheckIfSaltTVNeedsUpdate</t>
-  </si>
-  <si>
-    <t>$flow.tv.app.WhatAppleTVcnxType</t>
-  </si>
-  <si>
-    <t>$flow.tv.app.IsIssueWithOtherApps</t>
-  </si>
-  <si>
-    <t>$flow.tv.app.CanCheckWithLan</t>
-  </si>
-  <si>
-    <t>$flow.tv.services.IsMessageInvitingToContactCC</t>
-  </si>
-  <si>
-    <t>$flow.tv.services.IsTVServicesActiveVTI</t>
-  </si>
-  <si>
-    <t>$flow.tv.services.IsBasicTvPackageVisible</t>
-  </si>
-  <si>
-    <t>$flow.tv.services.IsBarringVisible</t>
-  </si>
-  <si>
-    <t>$flow.tv._OpenSaltTVApp</t>
-  </si>
-  <si>
-    <t>$flow.tv.CanExploreMenu</t>
-  </si>
-  <si>
-    <t>$flow.tv._InformSaltIsFixing</t>
-  </si>
-  <si>
-    <t>Can you explore the Salt TV menu ?</t>
-  </si>
-  <si>
-    <t>Channel issue = I cannot play a channel&lt;N&gt; Feature issue some app funcitonality doesn not work</t>
-  </si>
-  <si>
-    <t>$flow.tv.ChekSaltTVKNownBugs</t>
-  </si>
-  <si>
-    <t>Yes there is incident</t>
-  </si>
-  <si>
-    <t>Our technician are fixing it.</t>
-  </si>
-  <si>
-    <t>Gently close the call. Aplologies for inconvienience</t>
-  </si>
-  <si>
-    <t>Check in VTI if the customer has basic packages</t>
-  </si>
-  <si>
-    <t>Check in VTI if any barring is visible</t>
-  </si>
-  <si>
-    <t>Is the Apple ID a swiss Apple ID ?</t>
-  </si>
-  <si>
-    <t>Is ok for you to change the country of your Apple ID to Swiss ?</t>
-  </si>
-  <si>
-    <t>Let's change your Apple ID country !</t>
-  </si>
-  <si>
-    <t>https://support.apple.com/en-us/HT201389</t>
-  </si>
-  <si>
-    <t>Customer can always revert to another country if needed later.&lt;N&gt;Read "What to do before you change your country or region" on the link below to know the conditions to change languges of an Apple ID</t>
-  </si>
-  <si>
-    <t>There are several ways one can change the language (On the iPhone, iPad, iPod touch, a Mac computer or ther ApplerID web page).&lt;N&gt;Here is the Apple ID web page:&lt;N&gt;On a web browser&lt;N&gt;&lt;T&gt;1. Sing in https://appleid.apple.com/ with your Apple ID&lt;N&gt;&lt;T&gt;2. Scroll to the Account section, then click Edit.&lt;N&gt;&lt;T&gt;From the Country/Region menu, select your new country or region.&lt;N&gt;&lt;T&gt;4. When asked if you want to change your country or region, click "Continue to update." &lt;N&gt;&lt;T&gt;</t>
-  </si>
-  <si>
-    <t>Does the issue occurs only with Salt TV or with other Apple TV apps?</t>
-  </si>
-  <si>
-    <t>Can you try connecting the Apple TV to the LAN ?</t>
-  </si>
-  <si>
-    <t>&lt;T&gt;- Check the account to analyse the status&lt;N&gt;&lt;T&gt;- Check if there isn't any ticket opened for this case&lt;N&gt;&lt;T&gt;- Check if there is no outstanding technical issue that could be the source of the issue</t>
-  </si>
-  <si>
-    <t>Remote</t>
-  </si>
-  <si>
-    <t>TV</t>
-  </si>
-  <si>
-    <t>Sound</t>
-  </si>
-  <si>
-    <t>With what do  you face issues ?</t>
-  </si>
-  <si>
-    <t>$flow.lan.LetsCheckYourWiFi</t>
-  </si>
-  <si>
-    <t>The LAN conexion work, let's test your WiFi</t>
-  </si>
-  <si>
-    <t>Have the customer open a browser on a WiFi connected device and try google.com</t>
-  </si>
-  <si>
-    <t>WiFi works too</t>
-  </si>
-  <si>
-    <t>Did not work</t>
-  </si>
-  <si>
-    <t>customer/google_wifi</t>
+    <t>The customer contacts us, complaining about&lt;N&gt;&lt;T&gt;- not being able to connect to the Internet&lt;N&gt;&lt;T&gt;- having trouble watching the TV.&lt;N&gt;&lt;T&gt;- hasn't received his equipment (Fiber Box).&lt;N&gt;&lt;N&gt;&lt;b&gt;To carry on with the troubleshooting, the customer must be at home and be able to physically acces the box&lt;b&gt;</t>
+  </si>
+  <si>
+    <t>Check google.com, try to search for something like "Salt" and see if results are displayed.&lt;N&gt;&lt;N&gt;If the customer is computer savvy, have him also double check if the operating system show that the Ethernet connexion is ok</t>
+  </si>
+  <si>
+    <t>If the customer has another device that he can connect in LAN, have him connect it directly to the box and the ethernet connection like before.</t>
+  </si>
+  <si>
+    <t>&lt;N&gt;&lt;T&gt;- Check the account to analyse the status&lt;N&gt;&lt;T&gt;- Check if there isn't any ticket opened for this case&lt;N&gt;&lt;T&gt;- Check if there is no outstanding technical issue that could be the source of the issue</t>
+  </si>
+  <si>
+    <t>Open the Salt page.&lt;N&gt;Review the functionalities with the customer&lt;N&gt;Send the link to the Salt Fiber Apple TV guide</t>
+  </si>
+  <si>
+    <t>Take the proof of purchase with you to a Salt Store.&lt;N&gt;The remote will be replaced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give the customer tips for an optimal WiFi connection:&lt;N&gt;&lt;T&gt;- regularly reboot your Fiber Box in order to allow the system to remain in a stable state and up to date (the latest firmware is downloaded when the Fiber Box starts).&lt;N&gt;&lt;T&gt;- to place the Fiber Box in a central location in your home.&lt;N&gt;&lt;T&gt;- not to place the Fiber Box behind, under, or on top of the TV set, next to a metal object or near an aquarium.&lt;N&gt;&lt;T&gt;- to place the Fiber Box horizontally and, if possible, high up.&lt;N&gt;&lt;T&gt;- to use Wi-Fi repeaters to cover areas far from your Fiber Box. </t>
+  </si>
+  <si>
+    <t>Ask the customer to open a browser and enter google.com&lt;N&gt;If he can reach it than no ticket will be created &lt;b&gt;unless the client states the url or app&lt;b&gt; that still doesn't work.</t>
+  </si>
+  <si>
+    <t>&lt;N&gt;&lt;T&gt;-Audio Output&lt;N&gt;&lt;T&gt;-Audio Format&lt;N&gt;&lt;T&gt;-Reduce Loud Sounds&lt;N&gt;&lt;T&gt;-Audio Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An Apple ID created by selecting a country other than Switzerland does not allow you to download Salt TV. </t>
+  </si>
+  <si>
+    <t>There are several ways one can change the language (On the iPhone, iPad, iPod touch, a Mac computer or ther Apple ID web page).&lt;N&gt;Here is the Apple ID web page:&lt;N&gt;On a web browser&lt;N&gt;&lt;T&gt;1. Sign in https://appleid.apple.com/ with your Apple ID&lt;N&gt;&lt;T&gt;2. Scroll to the Account section, then click Edit.&lt;N&gt;&lt;T&gt;3. From the Country/Region menu, select your new country or region.&lt;N&gt;&lt;T&gt;4. When asked if you want to change your country or region, click "Continue to update."</t>
+  </si>
+  <si>
+    <t>End the call politely. Apologize for the inconvenience.</t>
   </si>
 </sst>
 </file>
@@ -2952,7 +2938,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2997,7 +2982,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3020,9 +3005,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3368,14 +3350,14 @@
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>604</v>
       </c>
@@ -3389,7 +3371,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>385</v>
       </c>
@@ -3397,7 +3379,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>417</v>
       </c>
@@ -3405,7 +3387,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>357</v>
       </c>
@@ -3433,19 +3415,19 @@
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="81.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3471,7 +3453,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -3479,7 +3461,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -3493,7 +3475,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -3504,7 +3486,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -3515,7 +3497,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -3526,10 +3508,10 @@
         <v>105</v>
       </c>
       <c r="D6" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>106</v>
       </c>
@@ -3537,13 +3519,13 @@
         <v>107</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -3560,7 +3542,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>113</v>
       </c>
@@ -3571,7 +3553,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -3579,7 +3561,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -3596,7 +3578,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>123</v>
       </c>
@@ -3610,7 +3592,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>127</v>
       </c>
@@ -3627,7 +3609,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>132</v>
       </c>
@@ -3641,7 +3623,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>136</v>
       </c>
@@ -3655,7 +3637,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -3672,7 +3654,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -3694,19 +3676,19 @@
       <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="72.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="72.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3732,7 +3714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -3743,7 +3725,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -3754,7 +3736,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -3771,7 +3753,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -3785,7 +3767,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -3799,7 +3781,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -3813,7 +3795,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>80</v>
       </c>
@@ -3824,7 +3806,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -3835,11 +3817,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="11" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>87</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -3867,23 +3849,23 @@
   </sheetPr>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="81.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3909,7 +3891,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3917,7 +3899,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -3925,7 +3907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3936,12 +3918,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -3952,7 +3934,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -3975,7 +3957,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -3986,7 +3968,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -4000,7 +3982,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -4017,12 +3999,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="9" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>842</v>
+        <v>878</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>39</v>
@@ -4040,7 +4022,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -4060,7 +4042,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>50</v>
       </c>
@@ -4068,7 +4050,7 @@
         <v>51</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>835</v>
+        <v>877</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>52</v>
@@ -4080,7 +4062,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -4091,15 +4073,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>58</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>743</v>
+        <v>881</v>
       </c>
       <c r="C15" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D15"/>
       <c r="E15"/>
@@ -4107,33 +4089,33 @@
       <c r="G15"/>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:8" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="7" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="C16" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="D16" t="s">
-        <v>672</v>
+        <v>665</v>
       </c>
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:3" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" s="11" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>883</v>
+      <c r="B17" s="1" t="s">
+        <v>881</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
   </sheetData>
@@ -4153,15 +4135,15 @@
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>604</v>
       </c>
@@ -4175,7 +4157,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>608</v>
       </c>
@@ -4189,7 +4171,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>385</v>
       </c>
@@ -4200,7 +4182,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>612</v>
       </c>
@@ -4208,7 +4190,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>614</v>
       </c>
@@ -4216,7 +4198,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>616</v>
       </c>
@@ -4224,7 +4206,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>618</v>
       </c>
@@ -4232,7 +4214,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>620</v>
       </c>
@@ -4240,7 +4222,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>622</v>
       </c>
@@ -4258,29 +4240,29 @@
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.109375" customWidth="1"/>
+    <col min="2" max="2" width="81.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="81.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -4302,731 +4284,767 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>886</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>867</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>839</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>746</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>750</v>
       </c>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="2" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>756</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B13" s="3" t="s">
+        <v>882</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="H13" s="14" t="s">
         <v>758</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    </row>
+    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>759</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="2" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>761</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="2" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>762</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>764</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    </row>
+    <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>765</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="2" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="2" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>767</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B19" s="3" t="s">
+        <v>868</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="H19" s="14" t="s">
         <v>768</v>
       </c>
-      <c r="C8" s="2" t="s">
+    </row>
+    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>769</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="B20" s="3"/>
+      <c r="C20" s="2" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>770</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="2" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>771</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B22" s="3"/>
+      <c r="C22" s="2" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>772</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="B23" s="3"/>
+      <c r="C23" s="2" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>773</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="B24" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>774</v>
       </c>
-      <c r="C10" s="2" t="s">
+    </row>
+    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>775</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="B25" s="3"/>
+      <c r="C25" s="2" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
         <v>776</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="B26" s="3" t="s">
+        <v>707</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
         <v>777</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="B27" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
         <v>778</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>780</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>783</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>781</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>784</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>786</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>788</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>789</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>791</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>792</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>793</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>795</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>798</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>796</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>799</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>801</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>803</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>805</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>807</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>809</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>810</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>812</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>715</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>716</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>717</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>718</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>813</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>696</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>697</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>698</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>814</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>736</v>
+      <c r="B28" s="3" t="s">
+        <v>727</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>737</v>
+        <v>728</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>738</v>
+        <v>729</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>739</v>
+        <v>730</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>135</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>815</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>674</v>
+        <v>731</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
+        <v>779</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>667</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>675</v>
+        <v>668</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>676</v>
+        <v>669</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>677</v>
+        <v>670</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>816</v>
-      </c>
-      <c r="B30" s="2" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>780</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
+        <v>781</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="2" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>869</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="2" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>887</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>706</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>707</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>817</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>723</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>724</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>718</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>818</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>819</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>831</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>821</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>834</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>833</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>822</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>712</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>875</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>713</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:8" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>823</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>879</v>
+        <v>787</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>871</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>876</v>
+        <v>861</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>824</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>880</v>
+        <v>788</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>888</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>825</v>
-      </c>
-      <c r="B39" s="2" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="9" t="s">
+        <v>789</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="9" t="s">
+        <v>790</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="2" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="9" t="s">
+        <v>791</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>684</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="9" t="s">
+        <v>792</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="9" t="s">
+        <v>804</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>693</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>694</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>826</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>827</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>691</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>828</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>709</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>710</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>852</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>700</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>701</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>853</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>729</v>
+    <row r="44" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="9" t="s">
+        <v>805</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>720</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>730</v>
+        <v>721</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>731</v>
+        <v>722</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>854</v>
-      </c>
-      <c r="B45" s="2" t="s">
+    <row r="45" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
+        <v>807</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="9" t="s">
+        <v>808</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="H47" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>680</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>681</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>855</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>703</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>704</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>856</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>683</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>684</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>685</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>681</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>857</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>732</v>
+    </row>
+    <row r="48" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="9" t="s">
+        <v>809</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>723</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>733</v>
+        <v>724</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>734</v>
+        <v>725</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>858</v>
-      </c>
+        <v>810</v>
+      </c>
+      <c r="B49" s="3"/>
       <c r="C49" s="2" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>859</v>
-      </c>
+        <v>811</v>
+      </c>
+      <c r="B50" s="3"/>
       <c r="C50" s="2" t="s">
-        <v>882</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>860</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>720</v>
+        <v>864</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="9" t="s">
+        <v>812</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>872</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>721</v>
+        <v>712</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>183</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>861</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>725</v>
+        <v>713</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="9" t="s">
+        <v>813</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>716</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>726</v>
+        <v>717</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>727</v>
+        <v>718</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>673</v>
+        <v>666</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>862</v>
-      </c>
+        <v>814</v>
+      </c>
+      <c r="B53" s="3"/>
       <c r="C53" s="2" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="2" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>873</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>863</v>
-      </c>
-      <c r="C54" s="2" t="s">
+      <c r="C55" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="2" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A57" s="9" t="s">
+        <v>820</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>817</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="2" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>874</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>749</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>747</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>745</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>746</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>864</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>869</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>687</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>688</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>870</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>689</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>865</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>868</v>
-      </c>
       <c r="C59" s="2" t="s">
-        <v>887</v>
+        <v>866</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>884</v>
+        <v>826</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>886</v>
+        <v>828</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>866</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>872</v>
+        <v>818</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>889</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>871</v>
+        <v>822</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="9" t="s">
+        <v>834</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>836</v>
       </c>
     </row>
   </sheetData>
@@ -5044,25 +5062,25 @@
   <sheetPr codeName="Sheet4">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="81.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5088,7 +5106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>529</v>
       </c>
@@ -5099,7 +5117,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>531</v>
       </c>
@@ -5110,7 +5128,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>534</v>
       </c>
@@ -5121,7 +5139,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>536</v>
       </c>
@@ -5138,7 +5156,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>541</v>
       </c>
@@ -5146,38 +5164,38 @@
         <v>542</v>
       </c>
       <c r="D6" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>543</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>544</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>545</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>845</v>
+        <v>879</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>546</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>547</v>
       </c>
@@ -5191,7 +5209,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>550</v>
       </c>
@@ -5199,7 +5217,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>552</v>
       </c>
@@ -5210,7 +5228,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>555</v>
       </c>
@@ -5224,7 +5242,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>559</v>
       </c>
@@ -5232,7 +5250,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>561</v>
       </c>
@@ -5246,7 +5264,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>565</v>
       </c>
@@ -5260,7 +5278,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>569</v>
       </c>
@@ -5268,7 +5286,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>571</v>
       </c>
@@ -5276,7 +5294,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>573</v>
       </c>
@@ -5287,7 +5305,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>576</v>
       </c>
@@ -5301,7 +5319,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>579</v>
       </c>
@@ -5312,7 +5330,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>582</v>
       </c>
@@ -5323,7 +5341,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>585</v>
       </c>
@@ -5331,13 +5349,13 @@
         <v>586</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>587</v>
       </c>
-      <c r="B23" s="14"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="11" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>588</v>
@@ -5349,19 +5367,19 @@
         <v>590</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>591</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>846</v>
+        <v>799</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>592</v>
       </c>
@@ -5375,7 +5393,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>596</v>
       </c>
@@ -5389,7 +5407,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>599</v>
       </c>
@@ -5403,126 +5421,84 @@
         <v>602</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>603</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>848</v>
+        <v>880</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>849</v>
+        <v>801</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>851</v>
+        <v>803</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
         <v>633</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="13" t="s">
+        <v>885</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>641</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>634</v>
+      </c>
+      <c r="F29" s="11" t="s">
         <v>642</v>
       </c>
-      <c r="C29" t="s">
-        <v>645</v>
-      </c>
-      <c r="D29"/>
-      <c r="E29" t="s">
-        <v>634</v>
-      </c>
-      <c r="F29" t="s">
-        <v>647</v>
-      </c>
-      <c r="G29" t="s">
-        <v>648</v>
-      </c>
-      <c r="H29"/>
-    </row>
-    <row r="30" spans="1:8" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="G29" s="11" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>635</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>643</v>
-      </c>
-      <c r="C30" t="s">
-        <v>646</v>
-      </c>
-      <c r="D30"/>
-      <c r="E30" t="s">
-        <v>636</v>
-      </c>
-      <c r="F30" t="s">
-        <v>637</v>
-      </c>
-      <c r="G30"/>
-      <c r="H30"/>
-    </row>
-    <row r="31" spans="1:8" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>633</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>642</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>645</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>634</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>635</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>841</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>837</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>893</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>838</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>839</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>888</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>890</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>889</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>893</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>891</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>892</v>
+      <c r="B30" s="6" t="s">
+        <v>798</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>833</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>830</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>833</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>832</v>
       </c>
     </row>
   </sheetData>
@@ -5536,25 +5512,25 @@
   <sheetPr codeName="Sheet5">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.140625" customWidth="1"/>
-    <col min="3" max="3" width="74.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.109375" customWidth="1"/>
+    <col min="3" max="3" width="74.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="81.140625" customWidth="1"/>
+    <col min="8" max="8" width="81.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5580,12 +5556,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>456</v>
       </c>
@@ -5599,7 +5575,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>460</v>
       </c>
@@ -5610,7 +5586,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>463</v>
       </c>
@@ -5618,7 +5594,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>465</v>
       </c>
@@ -5635,13 +5611,13 @@
         <v>469</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>470</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -5649,7 +5625,7 @@
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>471</v>
       </c>
@@ -5657,7 +5633,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>473</v>
       </c>
@@ -5674,7 +5650,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>478</v>
       </c>
@@ -5688,7 +5664,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>482</v>
       </c>
@@ -5702,7 +5678,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>486</v>
       </c>
@@ -5716,7 +5692,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>490</v>
       </c>
@@ -5727,7 +5703,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>493</v>
       </c>
@@ -5741,7 +5717,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>497</v>
       </c>
@@ -5758,7 +5734,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>502</v>
       </c>
@@ -5775,7 +5751,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>507</v>
       </c>
@@ -5786,7 +5762,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>510</v>
       </c>
@@ -5794,7 +5770,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>512</v>
       </c>
@@ -5814,7 +5790,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>518</v>
       </c>
@@ -5825,15 +5801,15 @@
         <v>520</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:8" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="B21" t="s">
-        <v>649</v>
-      </c>
-      <c r="C21" t="s">
-        <v>652</v>
+      <c r="B21" s="3" t="s">
+        <v>884</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>645</v>
       </c>
       <c r="D21"/>
       <c r="E21"/>
@@ -5841,12 +5817,12 @@
       <c r="G21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>522</v>
       </c>
-      <c r="B22" t="s">
-        <v>650</v>
+      <c r="B22" s="12" t="s">
+        <v>876</v>
       </c>
       <c r="C22" t="s">
         <v>523</v>
@@ -5857,7 +5833,7 @@
       <c r="G22"/>
       <c r="H22"/>
     </row>
-    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>524</v>
       </c>
@@ -5877,53 +5853,9 @@
       </c>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>521</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>649</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>650</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>523</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>843</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>524</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>525</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>526</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>527</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>528</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5936,19 +5868,19 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="81.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5974,7 +5906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>328</v>
       </c>
@@ -5988,7 +5920,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>332</v>
       </c>
@@ -5996,7 +5928,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>334</v>
       </c>
@@ -6013,7 +5945,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>337</v>
       </c>
@@ -6030,7 +5962,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>342</v>
       </c>
@@ -6038,24 +5970,24 @@
         <v>343</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>344</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>346</v>
       </c>
@@ -6066,7 +5998,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>349</v>
       </c>
@@ -6086,7 +6018,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>353</v>
       </c>
@@ -6100,7 +6032,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>357</v>
       </c>
@@ -6120,7 +6052,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>361</v>
       </c>
@@ -6131,7 +6063,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>364</v>
       </c>
@@ -6148,7 +6080,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>369</v>
       </c>
@@ -6156,7 +6088,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>371</v>
       </c>
@@ -6167,7 +6099,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>374</v>
       </c>
@@ -6181,7 +6113,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>378</v>
       </c>
@@ -6189,15 +6121,15 @@
         <v>379</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>380</v>
       </c>
       <c r="B18" t="s">
-        <v>670</v>
+        <v>663</v>
       </c>
       <c r="C18" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
       <c r="D18" t="s">
         <v>381</v>
@@ -6212,7 +6144,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>385</v>
       </c>
@@ -6235,7 +6167,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>392</v>
       </c>
@@ -6252,7 +6184,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>397</v>
       </c>
@@ -6272,7 +6204,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>403</v>
       </c>
@@ -6286,7 +6218,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>407</v>
       </c>
@@ -6297,7 +6229,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>410</v>
       </c>
@@ -6311,7 +6243,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>414</v>
       </c>
@@ -6322,7 +6254,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>417</v>
       </c>
@@ -6348,7 +6280,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>425</v>
       </c>
@@ -6359,7 +6291,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>427</v>
       </c>
@@ -6376,7 +6308,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>431</v>
       </c>
@@ -6393,7 +6325,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>432</v>
       </c>
@@ -6407,7 +6339,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>436</v>
       </c>
@@ -6415,7 +6347,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>438</v>
       </c>
@@ -6423,12 +6355,12 @@
         <v>439</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>440</v>
       </c>
       <c r="B33" t="s">
-        <v>836</v>
+        <v>793</v>
       </c>
       <c r="C33" t="s">
         <v>441</v>
@@ -6443,7 +6375,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>445</v>
       </c>
@@ -6454,13 +6386,13 @@
         <v>447</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>448</v>
       </c>
       <c r="B35"/>
       <c r="C35" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="D35" t="s">
         <v>449</v>
@@ -6470,12 +6402,12 @@
       <c r="G35"/>
       <c r="H35"/>
     </row>
-    <row r="36" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>450</v>
       </c>
       <c r="B36" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
       <c r="C36" t="s">
         <v>451</v>
@@ -6485,7 +6417,7 @@
         <v>452</v>
       </c>
       <c r="F36" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="G36" t="s">
         <v>453</v>
@@ -6494,23 +6426,23 @@
         <v>352</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>448</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" s="11" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>450</v>
       </c>
-      <c r="B38" s="13" t="s">
-        <v>653</v>
+      <c r="B38" s="12" t="s">
+        <v>646</v>
       </c>
       <c r="C38" s="11" t="s">
         <v>451</v>
@@ -6519,7 +6451,7 @@
         <v>452</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="G38" s="11" t="s">
         <v>453</v>
@@ -6543,19 +6475,19 @@
       <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="81.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6581,7 +6513,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>278</v>
       </c>
@@ -6595,7 +6527,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>282</v>
       </c>
@@ -6609,7 +6541,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>286</v>
       </c>
@@ -6620,7 +6552,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>289</v>
       </c>
@@ -6631,7 +6563,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>292</v>
       </c>
@@ -6645,7 +6577,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>296</v>
       </c>
@@ -6653,10 +6585,10 @@
         <v>297</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>298</v>
       </c>
@@ -6670,7 +6602,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>302</v>
       </c>
@@ -6681,7 +6613,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>305</v>
       </c>
@@ -6695,7 +6627,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>309</v>
       </c>
@@ -6712,7 +6644,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>314</v>
       </c>
@@ -6723,7 +6655,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>317</v>
       </c>
@@ -6737,7 +6669,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>319</v>
       </c>
@@ -6751,7 +6683,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>323</v>
       </c>
@@ -6759,12 +6691,12 @@
         <v>324</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>325</v>
       </c>
       <c r="B16" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
       <c r="C16" t="s">
         <v>326</v>
@@ -6779,12 +6711,12 @@
       </c>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>325</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>326</v>
@@ -6810,18 +6742,18 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="70.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="70.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6847,7 +6779,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>218</v>
       </c>
@@ -6861,7 +6793,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>221</v>
       </c>
@@ -6878,7 +6810,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>225</v>
       </c>
@@ -6889,7 +6821,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>228</v>
       </c>
@@ -6906,7 +6838,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>233</v>
       </c>
@@ -6917,7 +6849,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>236</v>
       </c>
@@ -6925,10 +6857,10 @@
         <v>237</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>238</v>
       </c>
@@ -6936,7 +6868,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>240</v>
       </c>
@@ -6950,7 +6882,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>244</v>
       </c>
@@ -6964,7 +6896,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>248</v>
       </c>
@@ -6981,7 +6913,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>252</v>
       </c>
@@ -6998,7 +6930,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>256</v>
       </c>
@@ -7015,7 +6947,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>260</v>
       </c>
@@ -7026,7 +6958,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>263</v>
       </c>
@@ -7037,7 +6969,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>266</v>
       </c>
@@ -7051,7 +6983,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>270</v>
       </c>
@@ -7065,7 +6997,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>273</v>
       </c>
@@ -7096,19 +7028,19 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="81.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7134,7 +7066,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -7148,7 +7080,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>150</v>
       </c>
@@ -7159,7 +7091,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>153</v>
       </c>
@@ -7170,7 +7102,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>156</v>
       </c>
@@ -7184,7 +7116,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>160</v>
       </c>
@@ -7195,15 +7127,15 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>163</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -7214,7 +7146,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>167</v>
       </c>
@@ -7222,7 +7154,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>169</v>
       </c>
@@ -7230,7 +7162,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>171</v>
       </c>
@@ -7241,7 +7173,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>174</v>
       </c>
@@ -7252,7 +7184,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>177</v>
       </c>
@@ -7260,7 +7192,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>179</v>
       </c>
@@ -7268,7 +7200,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>181</v>
       </c>
@@ -7282,7 +7214,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>185</v>
       </c>
@@ -7299,7 +7231,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>190</v>
       </c>
@@ -7319,7 +7251,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>195</v>
       </c>
@@ -7327,7 +7259,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>197</v>
       </c>
@@ -7335,7 +7267,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>199</v>
       </c>
@@ -7346,7 +7278,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>202</v>
       </c>
@@ -7360,7 +7292,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>206</v>
       </c>
@@ -7380,7 +7312,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>211</v>
       </c>
@@ -7394,7 +7326,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>215</v>
       </c>

</xml_diff>